<commit_message>
enh: shear study t=1.016
</commit_message>
<xml_diff>
--- a/multiaxial_plate_optimization/results.xlsx
+++ b/multiaxial_plate_optimization/results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\compositeoptimization\multiaxial_plate_optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D7C4C8-6E6C-49A7-BF76-0BF6BCB4FAE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE1DBAC-49DD-419F-A3E0-3FDD6D1B19C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{FE7EAB9A-19C3-4E00-A1FE-7D328C08052D}"/>
+    <workbookView xWindow="-18666" yWindow="2405" windowWidth="18775" windowHeight="10066" xr2:uid="{FE7EAB9A-19C3-4E00-A1FE-7D328C08052D}"/>
   </bookViews>
   <sheets>
     <sheet name="article_verification" sheetId="1" r:id="rId1"/>
+    <sheet name="shear_ratio_study" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
   <si>
     <t>t = 1.016</t>
   </si>
@@ -50,15 +51,29 @@
   <si>
     <t>lambda crit (lb/in)</t>
   </si>
+  <si>
+    <t>Max error</t>
+  </si>
+  <si>
+    <t>Complete reproduction in 4 min 45s</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="174" formatCode="0.0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,15 +99,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -129,9 +147,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.15915887716257468"/>
-          <c:y val="9.5182770776656517E-2"/>
+          <c:y val="0.10178640634001968"/>
           <c:w val="0.8143646967665884"/>
-          <c:h val="0.84391614409452431"/>
+          <c:h val="0.83731254242082431"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1307,8 +1325,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3105509" y="336431"/>
-          <a:ext cx="10669489" cy="6839905"/>
+          <a:off x="4159455" y="337952"/>
+          <a:ext cx="10632952" cy="6897754"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1353,6 +1371,144 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>59721</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>165893</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>311878</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>59721</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Elipse 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CCEAC6A-50F0-F451-72A3-F52A9B886E17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7438624" y="2315861"/>
+          <a:ext cx="875913" cy="789648"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>265428</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>46450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1194943" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="CaixaDeTexto 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B7AE969-7D83-F98D-146C-E9514D524515}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8268087" y="2017254"/>
+          <a:ext cx="1194943" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t>319.5 against 330</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Max error</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t> = 3.2</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>%</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1653,10 +1809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4B8029-BC16-4C1F-924A-45DA5A5A793C}">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1664,19 +1820,23 @@
     <col min="1" max="1" width="10.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1687,7 +1847,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -1699,7 +1859,7 @@
         <v>21.727952923549829</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.5</v>
       </c>
@@ -1711,7 +1871,7 @@
         <v>11.831641273671636</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -1723,7 +1883,7 @@
         <v>7.7814704900158649</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1.5</v>
       </c>
@@ -1735,7 +1895,7 @@
         <v>5.7970415963392004</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -1747,7 +1907,7 @@
         <v>4.6190864558819191</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2.5</v>
       </c>
@@ -1759,29 +1919,29 @@
         <v>3.8390022997561348</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1792,7 +1952,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>0</v>
       </c>
@@ -1804,7 +1964,7 @@
         <v>73.331841116980399</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0.5</v>
       </c>
@@ -1974,25 +2134,25 @@
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>5</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -2003,7 +2163,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>0</v>
       </c>
@@ -2014,8 +2174,11 @@
         <f t="shared" si="0"/>
         <v>586.65472893583637</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>0.5</v>
       </c>
@@ -2026,8 +2189,12 @@
         <f t="shared" si="0"/>
         <v>319.45441442921287</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="2">
+        <f>(330-319.5)/330</f>
+        <v>3.1818181818181815E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>1</v>
       </c>
@@ -2039,7 +2206,7 @@
         <v>210.09971365546062</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>1.5</v>
       </c>
@@ -2051,7 +2218,7 @@
         <v>156.52018347002812</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2</v>
       </c>
@@ -2063,7 +2230,7 @@
         <v>124.71533666737555</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2.5</v>
       </c>
@@ -2075,22 +2242,22 @@
         <v>103.65306405646014</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
@@ -2143,4 +2310,16 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50ED49A0-D37A-4577-88F6-A8D17B768348}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
enh: shear study with t=3.048
</commit_message>
<xml_diff>
--- a/multiaxial_plate_optimization/results.xlsx
+++ b/multiaxial_plate_optimization/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\compositeoptimization\multiaxial_plate_optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE1DBAC-49DD-419F-A3E0-3FDD6D1B19C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DECF5A-C4EA-4969-9284-D0E4788E8D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18666" yWindow="2405" windowWidth="18775" windowHeight="10066" xr2:uid="{FE7EAB9A-19C3-4E00-A1FE-7D328C08052D}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="1" xr2:uid="{FE7EAB9A-19C3-4E00-A1FE-7D328C08052D}"/>
   </bookViews>
   <sheets>
     <sheet name="article_verification" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="20">
   <si>
     <t>t = 1.016</t>
   </si>
@@ -56,6 +56,36 @@
   </si>
   <si>
     <t>Complete reproduction in 4 min 45s</t>
+  </si>
+  <si>
+    <t>T = 1.016</t>
+  </si>
+  <si>
+    <t>shear_ratio = 0</t>
+  </si>
+  <si>
+    <t>shear_ratio = 0.5</t>
+  </si>
+  <si>
+    <t>shear_ratio = 1.0</t>
+  </si>
+  <si>
+    <t>shear_ratio = 2.0</t>
+  </si>
+  <si>
+    <t>shear_ratio = 2.5</t>
+  </si>
+  <si>
+    <t>shear_ratio = 3.0</t>
+  </si>
+  <si>
+    <t>shear_ratio = 3.5</t>
+  </si>
+  <si>
+    <t>shear_ratio = 4.0</t>
+  </si>
+  <si>
+    <t>T = 3.048</t>
   </si>
 </sst>
 </file>
@@ -103,10 +133,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,6 +764,1988 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>shear_ratio_study!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>shear_ratio = 0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$A$4:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$B$4:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.8051457358475398</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0720368595381502</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.36274362146328</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0152170427607501</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.80892558966892603</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.67231198825959704</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8ADA-47FD-A134-41E6ED519A5C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>shear_ratio_study!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>shear_ratio = 0.5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$A$13:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$B$13:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.4600061212738802</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0154054759972602</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3469992189287401</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.00875029899985</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.80566011317541697</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.67043768734314502</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8ADA-47FD-A134-41E6ED519A5C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>shear_ratio_study!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>shear_ratio = 1.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$A$22:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$B$22:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.8563442951865698</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.86921703518209</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3024751182693499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98995342284552301</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.79605685785312097</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.66489140340726804</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8ADA-47FD-A134-41E6ED519A5C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>shear_ratio_study!$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>shear_ratio = 2.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$A$31:$A$36</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$B$31:$B$36</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.97813785285584</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5117872742671099</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.16110892178152</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.92381463535619401</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.76061670223633504</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.64389873071261905</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-8ADA-47FD-A134-41E6ED519A5C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>shear_ratio_study!$A$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>shear_ratio = 2.5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$A$40:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$B$40:$B$45</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.6990812901811601</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.35723705709562</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0831611469234499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.88252835663497797</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.73700467930983005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.62938939930534799</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-8ADA-47FD-A134-41E6ED519A5C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>shear_ratio_study!$A$47</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>shear_ratio = 3.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$A$49:$A$54</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$B$49:$B$54</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.4846702696110601</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2257444946704099</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.00844039103768</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.83957173105266103</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.71115115595182399</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61298940063852103</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-8ADA-47FD-A134-41E6ED519A5C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>shear_ratio_study!$A$56</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>shear_ratio = 3.5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$A$58:$A$63</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$B$58:$B$63</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.3168355179749001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.11464818315745</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93937281769941705</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.79693445884072001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.68418438512434898</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.59530272659085604</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-8ADA-47FD-A134-41E6ED519A5C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>shear_ratio_study!$A$65</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>shear_ratio = 4.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$A$67:$A$72</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$B$67:$B$72</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.18260880303153</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0204857528451901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.87670583034451599</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75586565368031899</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.65699648786106501</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.57687273392924698</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-8ADA-47FD-A134-41E6ED519A5C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="628333720"/>
+        <c:axId val="628332280"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="628333720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="628332280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="628332280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="628333720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>shear_ratio_study!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>shear_ratio = 0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$D$4:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$E$4:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>102.738934867886</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55.945012872786897</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36.794079525118001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.410870722909898</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.840991328848901</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.152424029155402</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D826-434D-BFE2-BEEEB429D833}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>shear_ratio_study!$D$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>shear_ratio = 0.5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$D$13:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$E$13:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>93.420165274385297</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54.415950854668701</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36.368979741973199</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.236263409090402</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.752826122530301</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.101817617749699</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D826-434D-BFE2-BEEEB429D833}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>shear_ratio_study!$D$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>shear_ratio = 1.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$D$22:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$E$22:$E$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>77.121295970035206</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50.4688602030418</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35.166831150860098</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.728742751436201</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.4935367691705</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.9520725405884</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D826-434D-BFE2-BEEEB429D833}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>shear_ratio_study!$D$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>shear_ratio = 2.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$D$31:$D$36</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$E$31:$E$36</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>53.409722027111698</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.818256776181798</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.3499413366299</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.942999194716101</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.536653843599701</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.385268200684301</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D826-434D-BFE2-BEEEB429D833}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>shear_ratio_study!$D$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>shear_ratio = 2.5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$D$40:$D$45</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$E$40:$E$45</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>45.875194834896803</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.645399998342398</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.245355536993099</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.828266754290699</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.899127672244401</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.993514074534399</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-D826-434D-BFE2-BEEEB429D833}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>shear_ratio_study!$D$47</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>shear_ratio = 3.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$D$49:$D$54</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$E$49:$E$54</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>40.086106941930801</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.095102802654502</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.2278915587402</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.668444800470301</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.2010816188338</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.550716519079799</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-D826-434D-BFE2-BEEEB429D833}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>shear_ratio_study!$D$56</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>shear_ratio = 3.5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$D$58:$D$63</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$E$58:$E$63</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>35.554560119060703</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.095502082772999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.363071054676901</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.5172322672814</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.472980584497002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.073173329844401</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-D826-434D-BFE2-BEEEB429D833}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>shear_ratio_study!$D$65</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>shear_ratio = 4.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$D$67:$D$72</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>shear_ratio_study!$E$67:$E$72</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>31.930439706561</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.553116225075701</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.671057462885901</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.4083732547798</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.738906118223699</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.5755670218243</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-D826-434D-BFE2-BEEEB429D833}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="628333720"/>
+        <c:axId val="628332280"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="628333720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="628332280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="628332280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="628333720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -773,7 +2786,1119 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1509,6 +4634,85 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>81951</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142335</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>306238</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>168214</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77559683-3C3F-C25D-01CE-A47A861312E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>215660</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>34505</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>439947</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>60385</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFFF961A-01A0-4C4C-9C05-86F8F6175BB1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1811,8 +5015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4B8029-BC16-4C1F-924A-45DA5A5A793C}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2314,12 +5518,931 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50ED49A0-D37A-4577-88F6-A8D17B768348}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R33" sqref="R33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3.8051457358475398</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>102.738934867886</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2.0720368595381502</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="3">
+        <v>55.945012872786897</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1.36274362146328</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>36.794079525118001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1.0152170427607501</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E7" s="3">
+        <v>27.410870722909898</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.80892558966892603</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>21.840991328848901</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.67231198825959704</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E9" s="3">
+        <v>18.152424029155402</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0</v>
+      </c>
+      <c r="B13" s="3">
+        <v>3.4600061212738802</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>93.420165274385297</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2.0154054759972602</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E14" s="3">
+        <v>54.415950854668701</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1.3469992189287401</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3">
+        <v>36.368979741973199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1.00875029899985</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E16" s="3">
+        <v>27.236263409090402</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>2</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.80566011317541697</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3">
+        <v>21.752826122530301</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.67043768734314502</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E18" s="3">
+        <v>18.101817617749699</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="3"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3">
+        <v>2.8563442951865698</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>77.121295970035206</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1.86921703518209</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E23" s="3">
+        <v>50.4688602030418</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1.3024751182693499</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3">
+        <v>35.166831150860098</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.98995342284552301</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E25" s="3">
+        <v>26.728742751436201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>2</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0.79605685785312097</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2</v>
+      </c>
+      <c r="E26" s="3">
+        <v>21.4935367691705</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.66489140340726804</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E27" s="3">
+        <v>17.9520725405884</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="3"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="D29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>0</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1.97813785285584</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3">
+        <v>53.409722027111698</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1.5117872742671099</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E32" s="3">
+        <v>40.818256776181798</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>1</v>
+      </c>
+      <c r="B33" s="3">
+        <v>1.16110892178152</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3">
+        <v>31.3499413366299</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="B34" s="3">
+        <v>0.92381463535619401</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E34" s="3">
+        <v>24.942999194716101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>2</v>
+      </c>
+      <c r="B35" s="3">
+        <v>0.76061670223633504</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2</v>
+      </c>
+      <c r="E35" s="3">
+        <v>20.536653843599701</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B36" s="3">
+        <v>0.64389873071261905</v>
+      </c>
+      <c r="D36" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E36" s="3">
+        <v>17.385268200684301</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="3"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="D38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>0</v>
+      </c>
+      <c r="B40" s="3">
+        <v>1.6990812901811601</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0</v>
+      </c>
+      <c r="E40" s="3">
+        <v>45.875194834896803</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1.35723705709562</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E41" s="3">
+        <v>36.645399998342398</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>1</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1.0831611469234499</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3">
+        <v>29.245355536993099</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="B43" s="3">
+        <v>0.88252835663497797</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E43" s="3">
+        <v>23.828266754290699</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>2</v>
+      </c>
+      <c r="B44" s="3">
+        <v>0.73700467930983005</v>
+      </c>
+      <c r="D44" s="1">
+        <v>2</v>
+      </c>
+      <c r="E44" s="3">
+        <v>19.899127672244401</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B45" s="3">
+        <v>0.62938939930534799</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E45" s="3">
+        <v>16.993514074534399</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="3"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="D47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>0</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1.4846702696110601</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0</v>
+      </c>
+      <c r="E49" s="3">
+        <v>40.086106941930801</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B50" s="3">
+        <v>1.2257444946704099</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E50" s="3">
+        <v>33.095102802654502</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>1</v>
+      </c>
+      <c r="B51" s="3">
+        <v>1.00844039103768</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1</v>
+      </c>
+      <c r="E51" s="3">
+        <v>27.2278915587402</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="B52" s="3">
+        <v>0.83957173105266103</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E52" s="3">
+        <v>22.668444800470301</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>2</v>
+      </c>
+      <c r="B53" s="3">
+        <v>0.71115115595182399</v>
+      </c>
+      <c r="D53" s="1">
+        <v>2</v>
+      </c>
+      <c r="E53" s="3">
+        <v>19.2010816188338</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B54" s="3">
+        <v>0.61298940063852103</v>
+      </c>
+      <c r="D54" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E54" s="3">
+        <v>16.550716519079799</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="3"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="D56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>0</v>
+      </c>
+      <c r="B58" s="3">
+        <v>1.3168355179749001</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0</v>
+      </c>
+      <c r="E58" s="3">
+        <v>35.554560119060703</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B59" s="3">
+        <v>1.11464818315745</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E59" s="3">
+        <v>30.095502082772999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>1</v>
+      </c>
+      <c r="B60" s="3">
+        <v>0.93937281769941705</v>
+      </c>
+      <c r="D60" s="1">
+        <v>1</v>
+      </c>
+      <c r="E60" s="3">
+        <v>25.363071054676901</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="B61" s="3">
+        <v>0.79693445884072001</v>
+      </c>
+      <c r="D61" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E61" s="3">
+        <v>21.5172322672814</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>2</v>
+      </c>
+      <c r="B62" s="3">
+        <v>0.68418438512434898</v>
+      </c>
+      <c r="D62" s="1">
+        <v>2</v>
+      </c>
+      <c r="E62" s="3">
+        <v>18.472980584497002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B63" s="3">
+        <v>0.59530272659085604</v>
+      </c>
+      <c r="D63" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E63" s="3">
+        <v>16.073173329844401</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+      <c r="B64" s="3"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65" s="3"/>
+      <c r="D65" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>0</v>
+      </c>
+      <c r="B67" s="3">
+        <v>1.18260880303153</v>
+      </c>
+      <c r="D67" s="1">
+        <v>0</v>
+      </c>
+      <c r="E67" s="3">
+        <v>31.930439706561</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B68" s="3">
+        <v>1.0204857528451901</v>
+      </c>
+      <c r="D68" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E68" s="3">
+        <v>27.553116225075701</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>1</v>
+      </c>
+      <c r="B69" s="3">
+        <v>0.87670583034451599</v>
+      </c>
+      <c r="D69" s="1">
+        <v>1</v>
+      </c>
+      <c r="E69" s="3">
+        <v>23.671057462885901</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="B70" s="3">
+        <v>0.75586565368031899</v>
+      </c>
+      <c r="D70" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E70" s="3">
+        <v>20.4083732547798</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>2</v>
+      </c>
+      <c r="B71" s="3">
+        <v>0.65699648786106501</v>
+      </c>
+      <c r="D71" s="1">
+        <v>2</v>
+      </c>
+      <c r="E71" s="3">
+        <v>17.738906118223699</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B72" s="3">
+        <v>0.57687273392924698</v>
+      </c>
+      <c r="D72" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E72" s="3">
+        <v>15.5755670218243</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
enh: shear loads study
</commit_message>
<xml_diff>
--- a/multiaxial_plate_optimization/results.xlsx
+++ b/multiaxial_plate_optimization/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\compositeoptimization\multiaxial_plate_optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DECF5A-C4EA-4969-9284-D0E4788E8D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C351FD5-A2B6-49D0-81AC-FF14B95EFA38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="1" xr2:uid="{FE7EAB9A-19C3-4E00-A1FE-7D328C08052D}"/>
   </bookViews>
@@ -5520,8 +5520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50ED49A0-D37A-4577-88F6-A8D17B768348}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R33" sqref="R33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
enh: stacking sequence check
</commit_message>
<xml_diff>
--- a/multiaxial_plate_optimization/results.xlsx
+++ b/multiaxial_plate_optimization/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\compositeoptimization\multiaxial_plate_optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C351FD5-A2B6-49D0-81AC-FF14B95EFA38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D27F2A-F971-4653-A384-86FFE3DA5B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="1" xr2:uid="{FE7EAB9A-19C3-4E00-A1FE-7D328C08052D}"/>
   </bookViews>
@@ -5520,7 +5520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50ED49A0-D37A-4577-88F6-A8D17B768348}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
enh: gurdal and haftka study written
</commit_message>
<xml_diff>
--- a/multiaxial_plate_optimization/results.xlsx
+++ b/multiaxial_plate_optimization/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\compositeoptimization\multiaxial_plate_optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B8FBDB-4980-4AED-B3C2-D7C10847E205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24E1201-AF5A-44AD-97EF-A3FB7CB1F9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="1" xr2:uid="{FE7EAB9A-19C3-4E00-A1FE-7D328C08052D}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{FE7EAB9A-19C3-4E00-A1FE-7D328C08052D}"/>
   </bookViews>
   <sheets>
     <sheet name="article_verification" sheetId="1" r:id="rId1"/>
@@ -904,8 +904,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1001,8 +1004,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1098,8 +1104,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1195,8 +1204,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1330,8 +1342,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR" sz="1200" b="1">
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:rPr>
                   <a:t>Nyy/Nxx</a:t>
                 </a:r>
@@ -1396,9 +1408,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="pt-BR"/>
@@ -1437,7 +1449,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1451,8 +1463,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR" sz="1200" b="1">
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:rPr>
                   <a:t>Max Buckling load (N/mm)</a:t>
                 </a:r>
@@ -1472,7 +1484,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1517,9 +1529,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="pt-BR"/>
@@ -1549,9 +1561,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.88105689107048835"/>
+          <c:x val="0.84416358475602649"/>
           <c:y val="6.8841311243549613E-2"/>
-          <c:w val="0.10472319043220843"/>
+          <c:w val="0.14161640945169504"/>
           <c:h val="0.16726468965493682"/>
         </c:manualLayout>
       </c:layout>
@@ -1577,9 +1589,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="pt-BR"/>
@@ -1675,8 +1687,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1686,11 +1701,11 @@
             <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="FF0000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1772,8 +1787,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1900,15 +1918,15 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR" sz="1200" b="1">
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:rPr>
                   <a:t>Nyy/Nxx</a:t>
                 </a:r>
@@ -1935,9 +1953,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="pt-BR"/>
@@ -1973,9 +1991,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="pt-BR"/>
@@ -2021,15 +2039,15 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR" sz="1200" b="1">
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:rPr>
                   <a:t>Max Buckling load (N/mm)</a:t>
                 </a:r>
@@ -2056,9 +2074,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="pt-BR"/>
@@ -2094,9 +2112,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="pt-BR"/>
@@ -2126,10 +2144,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.88105689107048835"/>
-          <c:y val="6.8841311243549613E-2"/>
-          <c:w val="0.10472319043220843"/>
-          <c:h val="0.16726468965493682"/>
+          <c:x val="0.74547679280227508"/>
+          <c:y val="6.8841311243549599E-2"/>
+          <c:w val="0.2242215621257358"/>
+          <c:h val="0.20372342333570767"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2154,9 +2172,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="pt-BR"/>
@@ -2252,8 +2270,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2349,8 +2370,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2360,11 +2386,15 @@
             <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="38100">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2477,15 +2507,15 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR" sz="1200" b="1">
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:rPr>
                   <a:t>Nyy/Nxx</a:t>
                 </a:r>
@@ -2512,9 +2542,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="pt-BR"/>
@@ -2550,9 +2580,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="pt-BR"/>
@@ -2599,15 +2629,15 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR" sz="1200" b="1">
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:rPr>
                   <a:t>Max Buckling load (N/mm)</a:t>
                 </a:r>
@@ -2634,9 +2664,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="pt-BR"/>
@@ -2672,9 +2702,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="pt-BR"/>
@@ -2704,10 +2734,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.88105689107048835"/>
+          <c:x val="0.74757856050059501"/>
           <c:y val="6.8841311243549613E-2"/>
-          <c:w val="0.10472319043220843"/>
-          <c:h val="0.16726468965493682"/>
+          <c:w val="0.23820152100210173"/>
+          <c:h val="0.22131138686236523"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2732,9 +2762,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="pt-BR"/>
@@ -8466,16 +8496,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>907850</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1132137</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>60892</xdr:rowOff>
+      <xdr:rowOff>147156</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>188745</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>490670</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>69517</xdr:rowOff>
+      <xdr:rowOff>155781</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9003,8 +9033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4B8029-BC16-4C1F-924A-45DA5A5A793C}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="R45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AM89" sqref="AM89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -9821,8 +9851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50ED49A0-D37A-4577-88F6-A8D17B768348}">
   <dimension ref="A1:Q72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView topLeftCell="A16" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
enh: lamination database written
</commit_message>
<xml_diff>
--- a/multiaxial_plate_optimization/results.xlsx
+++ b/multiaxial_plate_optimization/results.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\compositeoptimization\multiaxial_plate_optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24E1201-AF5A-44AD-97EF-A3FB7CB1F9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B686020B-7B76-4195-A7FC-1C1CC50AFC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{FE7EAB9A-19C3-4E00-A1FE-7D328C08052D}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="1" xr2:uid="{FE7EAB9A-19C3-4E00-A1FE-7D328C08052D}"/>
   </bookViews>
   <sheets>
-    <sheet name="article_verification" sheetId="1" r:id="rId1"/>
-    <sheet name="shear_ratio_study" sheetId="2" r:id="rId2"/>
+    <sheet name="Performance" sheetId="3" r:id="rId1"/>
+    <sheet name="article_verification" sheetId="1" r:id="rId2"/>
+    <sheet name="shear_ratio_study" sheetId="2" r:id="rId3"/>
+    <sheet name="LP database" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="59">
   <si>
     <t>t = 1.016</t>
   </si>
@@ -180,6 +182,30 @@
   <si>
     <t>Extremos, pura compressão e puro shear</t>
   </si>
+  <si>
+    <t>Reproduction of Gurdal and haftka</t>
+  </si>
+  <si>
+    <t>Total runtime 4m 44.3 s</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>xi1</t>
+  </si>
+  <si>
+    <t>xi3</t>
+  </si>
+  <si>
+    <t>buckling load</t>
+  </si>
+  <si>
+    <t>nev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total </t>
+  </si>
 </sst>
 </file>
 
@@ -226,13 +252,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1639,6 +1680,7 @@
     <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -8278,6 +8320,55 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>16392</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>146650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>274840</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>151014</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7763F0CD-A34A-D046-D852-621A490BB516}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5606309" y="690114"/>
+          <a:ext cx="7090569" cy="4170923"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>526211</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -8608,10 +8699,229 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1477742</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>45008</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1019190" cy="280205"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="CaixaDeTexto 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B1DFF3B-EC38-036E-E070-25E09CB3F21D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4485735" y="12106986"/>
+          <a:ext cx="1019190" cy="280205"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>error of 3.2%</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.25665</cdr:x>
+      <cdr:y>0.42694</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.33598</cdr:x>
+      <cdr:y>0.52575</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="Elipse 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CCEAC6A-50F0-F451-72A3-F52A9B886E17}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2031979" y="2463272"/>
+          <a:ext cx="628097" cy="570093"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rtlCol="0" anchor="t"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8723,6 +9033,187 @@
         <a:xfrm>
           <a:off x="8971472" y="2911232"/>
           <a:ext cx="3329664" cy="680119"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600152</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>177459</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>273678</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>49295</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A942E73-C411-BF37-D4CD-6B531C211CD0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="600152" y="362310"/>
+          <a:ext cx="6451423" cy="5047686"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>66203</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>40667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>239073</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>27823</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FC2E8DF-929F-3E53-B820-C3A12DD653E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7460273" y="410370"/>
+          <a:ext cx="6334596" cy="4978154"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>406673</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>86262</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>391357</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>107664</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagem 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76C47E8F-F7BA-820D-ED87-066894320C16}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="406673" y="5631815"/>
+          <a:ext cx="6762581" cy="5197250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>71525</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>24646</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>480614</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>7092</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagem 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{225EC8CE-F6E0-DC69-0A23-D8E1642528FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7465595" y="5755050"/>
+          <a:ext cx="6570815" cy="4973443"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9030,11 +9521,523 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C99918-8F97-469B-B85F-9CAF676E3B72}">
+  <dimension ref="A1:F30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>1.016</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8">
+        <v>5.0000000000234597E-5</v>
+      </c>
+      <c r="D6" s="8">
+        <v>-0.999999999999998</v>
+      </c>
+      <c r="E6" s="9">
+        <v>-3.8051457358475398</v>
+      </c>
+      <c r="F6" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="8">
+        <v>-0.47913233359219798</v>
+      </c>
+      <c r="D7" s="8">
+        <v>-4.1835332815604101E-2</v>
+      </c>
+      <c r="E7" s="9">
+        <v>-2.0720368588006499</v>
+      </c>
+      <c r="F7" s="7">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8">
+        <v>-0.74205514036764897</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.484010280735298</v>
+      </c>
+      <c r="E8" s="9">
+        <v>-1.36274362145655</v>
+      </c>
+      <c r="F8" s="7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="C9" s="8">
+        <v>-0.87087837929469902</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.74165675858939994</v>
+      </c>
+      <c r="E9" s="9">
+        <v>-1.01521704281647</v>
+      </c>
+      <c r="F9" s="7">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="7">
+        <v>2</v>
+      </c>
+      <c r="C10" s="8">
+        <v>-0.947346669793526</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.894593339587053</v>
+      </c>
+      <c r="E10" s="9">
+        <v>-0.80892558968183903</v>
+      </c>
+      <c r="F10" s="7">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="C11" s="8">
+        <v>-0.99798695751447897</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.99587391502895795</v>
+      </c>
+      <c r="E11" s="9">
+        <v>-0.67231198825938299</v>
+      </c>
+      <c r="F11" s="7">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>1.524</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8">
+        <v>5.0000000000418999E-5</v>
+      </c>
+      <c r="D12" s="8">
+        <v>-0.999999999999998</v>
+      </c>
+      <c r="E12" s="9">
+        <v>-12.8423668584854</v>
+      </c>
+      <c r="F12" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="8">
+        <v>-0.47913165808486102</v>
+      </c>
+      <c r="D13" s="8">
+        <v>-4.1836683830281003E-2</v>
+      </c>
+      <c r="E13" s="9">
+        <v>-6.9931266099889404</v>
+      </c>
+      <c r="F13" s="7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="7">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8">
+        <v>-0.74205534113545002</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.484010682270891</v>
+      </c>
+      <c r="E14" s="9">
+        <v>-4.5992600260486904</v>
+      </c>
+      <c r="F14" s="7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="C15" s="8">
+        <v>-0.87087797974455206</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.74165595948909901</v>
+      </c>
+      <c r="E15" s="9">
+        <v>-3.4263583043562198</v>
+      </c>
+      <c r="F15" s="7">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="7">
+        <v>2</v>
+      </c>
+      <c r="C16" s="8">
+        <v>-0.94734640617969301</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0.89459281235938803</v>
+      </c>
+      <c r="E16" s="9">
+        <v>-2.7301236404857998</v>
+      </c>
+      <c r="F16" s="7">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="C17" s="8">
+        <v>-0.99798688814339997</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.99587377628680096</v>
+      </c>
+      <c r="E17" s="9">
+        <v>-2.26905291199777</v>
+      </c>
+      <c r="F17" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>2.032</v>
+      </c>
+      <c r="B18" s="7">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8">
+        <v>4.9999999998434997E-5</v>
+      </c>
+      <c r="D18" s="8">
+        <v>-0.999999999999998</v>
+      </c>
+      <c r="E18" s="9">
+        <v>-30.441165886780599</v>
+      </c>
+      <c r="F18" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C19" s="8">
+        <v>-0.47913158805508399</v>
+      </c>
+      <c r="D19" s="8">
+        <v>-4.1836823889845401E-2</v>
+      </c>
+      <c r="E19" s="9">
+        <v>-16.576300415339301</v>
+      </c>
+      <c r="F19" s="7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="7">
+        <v>1</v>
+      </c>
+      <c r="C20" s="8">
+        <v>-0.742055284810055</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0.48401056962012401</v>
+      </c>
+      <c r="E20" s="9">
+        <v>-10.9019494969431</v>
+      </c>
+      <c r="F20" s="7">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="C21" s="8">
+        <v>-0.87087769319643005</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0.74165538639287698</v>
+      </c>
+      <c r="E21" s="9">
+        <v>-8.1217395165769695</v>
+      </c>
+      <c r="F21" s="7">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="7">
+        <v>2</v>
+      </c>
+      <c r="C22" s="8">
+        <v>-0.94734670742802196</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0.89459341485606703</v>
+      </c>
+      <c r="E22" s="9">
+        <v>-6.4714047934906302</v>
+      </c>
+      <c r="F22" s="7">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="C23" s="8">
+        <v>-0.99798709067145996</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0.99587418134293504</v>
+      </c>
+      <c r="E23" s="9">
+        <v>-5.3784961261883604</v>
+      </c>
+      <c r="F23" s="7">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>3.048</v>
+      </c>
+      <c r="B24" s="7">
+        <v>0</v>
+      </c>
+      <c r="C24" s="8">
+        <v>4.9999999968861702E-5</v>
+      </c>
+      <c r="D24" s="8">
+        <v>-1</v>
+      </c>
+      <c r="E24" s="9">
+        <v>-102.738934867884</v>
+      </c>
+      <c r="F24" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C25" s="8">
+        <v>-0.47913166123825801</v>
+      </c>
+      <c r="D25" s="8">
+        <v>-4.1836677524023203E-2</v>
+      </c>
+      <c r="E25" s="9">
+        <v>-55.945012797327202</v>
+      </c>
+      <c r="F25" s="7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="7">
+        <v>1</v>
+      </c>
+      <c r="C26" s="8">
+        <v>-0.74205528265109799</v>
+      </c>
+      <c r="D26" s="8">
+        <v>0.48401056539334197</v>
+      </c>
+      <c r="E26" s="9">
+        <v>-36.794079525528304</v>
+      </c>
+      <c r="F26" s="7">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="C27" s="8">
+        <v>-0.87087769134662796</v>
+      </c>
+      <c r="D27" s="8">
+        <v>0.74165538269318299</v>
+      </c>
+      <c r="E27" s="9">
+        <v>-27.4108708522303</v>
+      </c>
+      <c r="F27" s="7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="7">
+        <v>2</v>
+      </c>
+      <c r="C28" s="8">
+        <v>-0.94734672787860597</v>
+      </c>
+      <c r="D28" s="8">
+        <v>0.89459345575695404</v>
+      </c>
+      <c r="E28" s="9">
+        <v>-21.840991317479599</v>
+      </c>
+      <c r="F28" s="7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="C29" s="8">
+        <v>-0.99798701868376705</v>
+      </c>
+      <c r="D29" s="8">
+        <v>0.99587403736817603</v>
+      </c>
+      <c r="E29" s="9">
+        <v>-18.152424024266399</v>
+      </c>
+      <c r="F29" s="7">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30">
+        <f>SUM(F6:F29)</f>
+        <v>1053</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="A24:A29"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4B8029-BC16-4C1F-924A-45DA5A5A793C}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AM89" sqref="AM89"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -9105,7 +10108,7 @@
         <v>3.5079523799999999</v>
       </c>
       <c r="F4" s="4">
-        <f>(B4-E4)/B4</f>
+        <f t="shared" ref="F4:F9" si="0">(B4-E4)/B4</f>
         <v>7.8103015358318331E-2</v>
       </c>
     </row>
@@ -9117,7 +10120,7 @@
         <v>2.0720368595696499</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" ref="C5:C42" si="0">B5*5.71015</f>
+        <f t="shared" ref="C5:C42" si="1">B5*5.71015</f>
         <v>11.831641273671636</v>
       </c>
       <c r="D5" t="s">
@@ -9127,7 +10130,7 @@
         <v>1.9293114200000001</v>
       </c>
       <c r="F5" s="4">
-        <f t="shared" ref="F5:F9" si="1">(B5-E5)/B5</f>
+        <f t="shared" si="0"/>
         <v>6.8881708793198312E-2</v>
       </c>
     </row>
@@ -9139,7 +10142,7 @@
         <v>1.3627436214488</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.7814704900158649</v>
       </c>
       <c r="D6" t="s">
@@ -9149,7 +10152,7 @@
         <v>1.1924668599999999</v>
       </c>
       <c r="F6" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.12495142796395589</v>
       </c>
     </row>
@@ -9161,7 +10164,7 @@
         <v>1.0152170426940099</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.7970415963392004</v>
       </c>
       <c r="D7" t="s">
@@ -9171,7 +10174,7 @@
         <v>0.85184291999999995</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.16092531530053472</v>
       </c>
     </row>
@@ -9183,7 +10186,7 @@
         <v>0.80892558967486305</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.6190864558819191</v>
       </c>
       <c r="D8" t="s">
@@ -9193,7 +10196,7 @@
         <v>0.59752698000000004</v>
       </c>
       <c r="F8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.26133257789487396</v>
       </c>
     </row>
@@ -9205,7 +10208,7 @@
         <v>0.67231198825882599</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.8390022997561348</v>
       </c>
       <c r="D9" t="s">
@@ -9215,7 +10218,7 @@
         <v>0.48888727999999998</v>
       </c>
       <c r="F9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.27282677010395856</v>
       </c>
     </row>
@@ -9272,7 +10275,7 @@
         <v>12.8423668584854</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>73.331841116980399</v>
       </c>
       <c r="D15" t="s">
@@ -9282,7 +10285,7 @@
         <v>11.707954790000001</v>
       </c>
       <c r="F15" s="4">
-        <f>(B15-E15)/B15</f>
+        <f t="shared" ref="F15:F20" si="2">(B15-E15)/B15</f>
         <v>8.8333566622561796E-2</v>
       </c>
     </row>
@@ -9294,7 +10297,7 @@
         <v>6.9931266100140999</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39.931801912172013</v>
       </c>
       <c r="D16" t="s">
@@ -9304,7 +10307,7 @@
         <v>6.6159842700000002</v>
       </c>
       <c r="F16" s="4">
-        <f t="shared" ref="F16:F20" si="2">(B16-E16)/B16</f>
+        <f t="shared" si="2"/>
         <v>5.3930432129461935E-2</v>
       </c>
     </row>
@@ -9316,7 +10319,7 @@
         <v>4.5992599985319202</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26.262464480617041</v>
       </c>
       <c r="D17" t="s">
@@ -9338,7 +10341,7 @@
         <v>3.4263583001996301</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.565019847884916</v>
       </c>
       <c r="D18" t="s">
@@ -9360,7 +10363,7 @@
         <v>2.73012364040894</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.589415505281108</v>
       </c>
       <c r="D19" t="s">
@@ -9382,7 +10385,7 @@
         <v>2.2690529119505198</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.956632485174261</v>
       </c>
       <c r="D20" t="s">
@@ -9449,7 +10452,7 @@
         <v>30.44116588</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>173.82362334968198</v>
       </c>
       <c r="D26" t="s">
@@ -9459,7 +10462,7 @@
         <v>29.585646239999999</v>
       </c>
       <c r="F26" s="4">
-        <f>(B26-E26)/B26</f>
+        <f t="shared" ref="F26:F31" si="3">(B26-E26)/B26</f>
         <v>2.8104036598745431E-2</v>
       </c>
     </row>
@@ -9471,7 +10474,7 @@
         <v>16.576299660832401</v>
       </c>
       <c r="C27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>94.653157508302129</v>
       </c>
       <c r="D27" t="s">
@@ -9481,7 +10484,7 @@
         <v>16.023814900000001</v>
       </c>
       <c r="F27" s="4">
-        <f t="shared" ref="F27:F31" si="3">(B27-E27)/B27</f>
+        <f t="shared" si="3"/>
         <v>3.3329800506553812E-2</v>
       </c>
     </row>
@@ -9493,7 +10496,7 @@
         <v>10.9019494969371</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>62.251766919935378</v>
       </c>
       <c r="D28" t="s">
@@ -9515,7 +10518,7 @@
         <v>8.1217395197936604</v>
       </c>
       <c r="C29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46.376350918949768</v>
       </c>
       <c r="D29" t="s">
@@ -9537,7 +10540,7 @@
         <v>6.4714047935697598</v>
       </c>
       <c r="C30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36.952692082002365</v>
       </c>
       <c r="D30" t="s">
@@ -9559,7 +10562,7 @@
         <v>5.3784961261037703</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30.71201965447144</v>
       </c>
       <c r="D31" t="s">
@@ -9629,7 +10632,7 @@
         <v>102.73893486788199</v>
       </c>
       <c r="C37" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>586.65472893583637</v>
       </c>
       <c r="D37" t="s">
@@ -9639,7 +10642,7 @@
         <v>94.643549969999995</v>
       </c>
       <c r="F37" s="4">
-        <f>(B37-E37)/B37</f>
+        <f t="shared" ref="F37:F42" si="4">(B37-E37)/B37</f>
         <v>7.8795686448300525E-2</v>
       </c>
       <c r="G37" t="s">
@@ -9654,7 +10657,7 @@
         <v>55.945012728074197</v>
       </c>
       <c r="C38" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>319.45441442921287</v>
       </c>
       <c r="D38" t="s">
@@ -9664,7 +10667,7 @@
         <v>53.382076929999997</v>
       </c>
       <c r="F38" s="4">
-        <f t="shared" ref="F38:F42" si="4">(B38-E38)/B38</f>
+        <f t="shared" si="4"/>
         <v>4.5811693895425165E-2</v>
       </c>
       <c r="G38" s="2">
@@ -9680,7 +10683,7 @@
         <v>36.794079604819601</v>
       </c>
       <c r="C39" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>210.09971365546062</v>
       </c>
       <c r="D39" t="s">
@@ -9702,7 +10705,7 @@
         <v>27.4108707249421</v>
       </c>
       <c r="C40" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>156.52018347002812</v>
       </c>
       <c r="D40" t="s">
@@ -9724,7 +10727,7 @@
         <v>21.840991334268899</v>
       </c>
       <c r="C41" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>124.71533666737555</v>
       </c>
       <c r="D41" t="s">
@@ -9746,7 +10749,7 @@
         <v>18.1524240267699</v>
       </c>
       <c r="C42" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>103.65306405646014</v>
       </c>
       <c r="D42" t="s">
@@ -9847,7 +10850,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50ED49A0-D37A-4577-88F6-A8D17B768348}">
   <dimension ref="A1:Q72"/>
   <sheetViews>
@@ -10779,4 +11782,19 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C8F2A27-AEE5-4E18-89CF-1EA204BCB0F1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="AC60" sqref="AC60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
enh: database study updates
</commit_message>
<xml_diff>
--- a/multiaxial_plate_optimization/results.xlsx
+++ b/multiaxial_plate_optimization/results.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\compositeoptimization\multiaxial_plate_optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B686020B-7B76-4195-A7FC-1C1CC50AFC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E137970-0146-4E2A-9FA2-EB7F04BEB802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="1" xr2:uid="{FE7EAB9A-19C3-4E00-A1FE-7D328C08052D}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="2" xr2:uid="{FE7EAB9A-19C3-4E00-A1FE-7D328C08052D}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="3" r:id="rId1"/>
     <sheet name="article_verification" sheetId="1" r:id="rId2"/>
-    <sheet name="shear_ratio_study" sheetId="2" r:id="rId3"/>
-    <sheet name="LP database" sheetId="4" r:id="rId4"/>
+    <sheet name="contour plots" sheetId="5" r:id="rId3"/>
+    <sheet name="shear_ratio_study" sheetId="2" r:id="rId4"/>
+    <sheet name="LP database" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="60">
   <si>
     <t>t = 1.016</t>
   </si>
@@ -205,6 +206,9 @@
   </si>
   <si>
     <t xml:space="preserve">total </t>
+  </si>
+  <si>
+    <t>r, xi1D, xi3D, nplies = 1.0, -0.74205514,  0.48401028, 8</t>
   </si>
 </sst>
 </file>
@@ -8369,16 +8373,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>526211</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>155276</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>69518</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>13192</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>15864</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>111302</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>178244</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>151896</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8401,7 +8405,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4159455" y="337952"/>
+          <a:off x="9335303" y="926577"/>
           <a:ext cx="10632952" cy="6897754"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8413,16 +8417,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>21563</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>25879</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>183942</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66473</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>491706</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>34506</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>35013</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>75100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8588,15 +8592,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1132137</xdr:colOff>
+      <xdr:colOff>1111840</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>147156</xdr:rowOff>
+      <xdr:rowOff>86264</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>490670</xdr:colOff>
+      <xdr:colOff>470373</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>155781</xdr:rowOff>
+      <xdr:rowOff>94889</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8923,6 +8927,1343 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>483080</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>25880</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>129396</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>75017</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90BABB51-D500-6DF2-343A-DEA8D18689BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="483080" y="1646146"/>
+          <a:ext cx="6494939" cy="4729905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>151175</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>84107</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>255339</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>10675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Elipse 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{599C7B1A-76EE-10AF-3D61-A4C2767CD16C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2014481" y="2827307"/>
+          <a:ext cx="104164" cy="109448"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>272019</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>10153</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>372120</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>119216</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Elipse 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{862132F5-9643-1948-538B-4A369DE16EB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2762428" y="2890625"/>
+          <a:ext cx="100101" cy="109063"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="002060"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="002060"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>437019</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>10153</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>540999</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>119216</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Elipse 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A29AF89-80E4-B3A5-913F-E6634918F308}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5417836" y="2890625"/>
+          <a:ext cx="103980" cy="109063"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="002060"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="002060"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>269466</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>146422</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>272019</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>64685</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Conector de Seta Reta 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E8E21CB-8A0F-DA41-9F6E-408F58BEDB1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="4" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2137272" y="2846865"/>
+          <a:ext cx="625156" cy="98292"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="002060"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>441776</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>101924</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="408966" cy="264560"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="CaixaDeTexto 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAB3ABE2-CC28-C121-9F68-2EB78C59840A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2309582" y="2622337"/>
+              <a:ext cx="408966" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="pt-BR" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑑</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑏𝑒𝑠𝑡</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="pt-BR" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="CaixaDeTexto 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAB3ABE2-CC28-C121-9F68-2EB78C59840A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2309582" y="2622337"/>
+              <a:ext cx="408966" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑑</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_𝑏𝑒𝑠𝑡</a:t>
+              </a:r>
+              <a:endParaRPr lang="pt-BR" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>622344</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>109157</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>39835</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>121055</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="CaixaDeTexto 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3D240A0-EC25-452B-F5B2-592DF7E70FF6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1244946" y="6590220"/>
+              <a:ext cx="1907899" cy="732016"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" i="0">
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>Best stack sequence</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="left"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="pt-BR" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <m:rPr>
+                            <m:nor/>
+                          </m:rPr>
+                          <a:rPr lang="pt-BR" sz="1100">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>[90/-45/0/45]</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="pt-BR" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑠</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="pt-BR" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="left"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:sSubSup>
+                          <m:sSubSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝜉</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>1</m:t>
+                            </m:r>
+                          </m:sub>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐷</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSubSup>
+                        <m:r>
+                          <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>, </m:t>
+                        </m:r>
+                        <m:sSubSup>
+                          <m:sSubSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝜉</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>3</m:t>
+                            </m:r>
+                          </m:sub>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="dk1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝐷</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSubSup>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−0.47, −0.37</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="pt-BR" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="CaixaDeTexto 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3D240A0-EC25-452B-F5B2-592DF7E70FF6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1244946" y="6590220"/>
+              <a:ext cx="1907899" cy="732016"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" i="0">
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>Best stack sequence</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>"[90/-45/0/45]</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>" 〗_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑠</a:t>
+              </a:r>
+              <a:endParaRPr lang="pt-BR" sz="1100"/>
+            </a:p>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(𝜉_1^𝐷, </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝜉_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>3</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>^𝐷</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> )</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>=(−0.47, −0.37)</a:t>
+              </a:r>
+              <a:endParaRPr lang="pt-BR" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>291514</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>160631</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>405067</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>45008</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Conector de Seta Reta 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B12139BF-005F-CEB3-D59B-5A47D05DB720}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2159320" y="2861074"/>
+          <a:ext cx="3226564" cy="64406"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="002060"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>10875</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>120046</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="504897" cy="264560"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14" name="CaixaDeTexto 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E08EF76-F06E-F67D-20A6-96D5CC2C9A6A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3746488" y="2640459"/>
+              <a:ext cx="504897" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="pt-BR" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑑</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑤𝑜𝑟𝑠𝑡</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="pt-BR" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14" name="CaixaDeTexto 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E08EF76-F06E-F67D-20A6-96D5CC2C9A6A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3746488" y="2640459"/>
+              <a:ext cx="504897" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑑</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_𝑤𝑜𝑟𝑠𝑡</a:t>
+              </a:r>
+              <a:endParaRPr lang="pt-BR" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>209776</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>90015</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>480078</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>173563</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="19" name="CaixaDeTexto 18">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFB42194-089D-8F43-3F9C-47C01E68BF26}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5813195" y="5130842"/>
+              <a:ext cx="892905" cy="623637"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" i="0">
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>8 plies</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="left"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑁</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑦𝑦</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:num>
+                      <m:den>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑁</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥𝑥</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="pt-BR" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=1</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="pt-BR" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="19" name="CaixaDeTexto 18">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFB42194-089D-8F43-3F9C-47C01E68BF26}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5813195" y="5130842"/>
+              <a:ext cx="892905" cy="623637"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" i="0">
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>8 plies</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑁_𝑦𝑦/𝑁_𝑥𝑥 =1</a:t>
+              </a:r>
+              <a:endParaRPr lang="pt-BR" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
@@ -9044,7 +10385,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -9525,7 +10866,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E8" sqref="B8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -10036,8 +11377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4B8029-BC16-4C1F-924A-45DA5A5A793C}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F6" sqref="B6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -10111,6 +11452,13 @@
         <f t="shared" ref="F4:F9" si="0">(B4-E4)/B4</f>
         <v>7.8103015358318331E-2</v>
       </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="5">
+        <f>AVERAGE(F4:F9)</f>
+        <v>0.16117013590247331</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -10133,6 +11481,7 @@
         <f t="shared" si="0"/>
         <v>6.8881708793198312E-2</v>
       </c>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -10288,6 +11637,13 @@
         <f t="shared" ref="F15:F20" si="2">(B15-E15)/B15</f>
         <v>8.8333566622561796E-2</v>
       </c>
+      <c r="G15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="5">
+        <f>AVERAGE(F15:F20)</f>
+        <v>4.5700033168451996E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -10311,7 +11667,7 @@
         <v>5.3930432129461935E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -10333,7 +11689,7 @@
         <v>5.5503490866070631E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1.5</v>
       </c>
@@ -10355,7 +11711,7 @@
         <v>6.8113075618128809E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -10377,7 +11733,7 @@
         <v>3.9474564013810443E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2.5</v>
       </c>
@@ -10399,22 +11755,22 @@
         <v>8.0099979596457829E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -10424,7 +11780,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -10444,7 +11800,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>0</v>
       </c>
@@ -10465,8 +11821,15 @@
         <f t="shared" ref="F26:F31" si="3">(B26-E26)/B26</f>
         <v>2.8104036598745431E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H26" s="5">
+        <f>AVERAGE(F26:F31)</f>
+        <v>3.4813963141702375E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>0.5</v>
       </c>
@@ -10488,7 +11851,7 @@
         <v>3.3329800506553812E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -10510,7 +11873,7 @@
         <v>9.9493817108191017E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1.5</v>
       </c>
@@ -10532,7 +11895,7 @@
         <v>4.1227292377159004E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2</v>
       </c>
@@ -10554,7 +11917,7 @@
         <v>2.8361658623508177E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2.5</v>
       </c>
@@ -10576,16 +11939,16 @@
         <v>6.7911609033428716E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -10594,7 +11957,7 @@
       </c>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -10604,7 +11967,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -10624,7 +11987,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>0</v>
       </c>
@@ -10646,10 +12009,14 @@
         <v>7.8795686448300525E-2</v>
       </c>
       <c r="G37" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="H37" s="5">
+        <f>AVERAGE(F37:F42)</f>
+        <v>9.1594768544536964E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>0.5</v>
       </c>
@@ -10670,12 +12037,8 @@
         <f t="shared" si="4"/>
         <v>4.5811693895425165E-2</v>
       </c>
-      <c r="G38" s="2">
-        <f>(330-319.5)/330</f>
-        <v>3.1818181818181815E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>1</v>
       </c>
@@ -10697,7 +12060,7 @@
         <v>4.4909719513765267E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>1.5</v>
       </c>
@@ -10719,7 +12082,7 @@
         <v>0.11557961316636697</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2</v>
       </c>
@@ -10741,7 +12104,7 @@
         <v>8.1364957161107004E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2.5</v>
       </c>
@@ -10763,19 +12126,19 @@
         <v>0.18310694108225684</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="F45" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="E46" t="s">
         <v>48</v>
@@ -10785,7 +12148,7 @@
         <v>8.3319725189291163E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="E47" t="s">
         <v>49</v>
@@ -10795,52 +12158,59 @@
         <v>7.2286098956684683E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <f>(330-319.5)/330</f>
+        <v>3.1818181818181815E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
     </row>
   </sheetData>
@@ -10851,6 +12221,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F647F3B3-630C-467F-BB9D-1DD7581BEBC2}">
+  <dimension ref="B4"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50ED49A0-D37A-4577-88F6-A8D17B768348}">
   <dimension ref="A1:Q72"/>
   <sheetViews>
@@ -11784,7 +13175,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C8F2A27-AEE5-4E18-89CF-1EA204BCB0F1}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
enh: added results for non balanced laminates
</commit_message>
<xml_diff>
--- a/multiaxial_plate_optimization/results.xlsx
+++ b/multiaxial_plate_optimization/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\compositeoptimization\multiaxial_plate_optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC4C5C6-E1C6-4681-BC85-E162654EF211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2617E1-68AE-47E0-8026-990D4615DD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18666" yWindow="2405" windowWidth="18775" windowHeight="10066" activeTab="1" xr2:uid="{FE7EAB9A-19C3-4E00-A1FE-7D328C08052D}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="1" xr2:uid="{FE7EAB9A-19C3-4E00-A1FE-7D328C08052D}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="3" r:id="rId1"/>
@@ -8453,15 +8453,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>59721</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>165893</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>130761</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>165894</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>311878</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>382919</xdr:colOff>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>59721</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -8477,8 +8477,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7438624" y="2315861"/>
-          <a:ext cx="875913" cy="789648"/>
+          <a:off x="12491907" y="2906049"/>
+          <a:ext cx="871230" cy="807212"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -8706,11 +8706,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1477742</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>45008</xdr:rowOff>
+      <xdr:colOff>1498039</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>20297</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1019190" cy="280205"/>
+    <xdr:ext cx="2023568" cy="655949"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="CaixaDeTexto 5">
@@ -8724,8 +8724,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4485735" y="12106986"/>
-          <a:ext cx="1019190" cy="280205"/>
+          <a:off x="4512210" y="12076981"/>
+          <a:ext cx="2023568" cy="655949"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8747,19 +8747,40 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
           <a:spAutoFit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="pt-BR" sz="1200" b="1">
+            <a:rPr lang="pt-BR" sz="1400" b="1">
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>error of 3.2%</a:t>
+            <a:t>max difference of +3.2% </a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>in comparison with Gurdal</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> and Haftka (1991)</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1200" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -9242,8 +9263,8 @@
       <xdr:rowOff>101924</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="408966" cy="264560"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="CaixaDeTexto 8">
@@ -9285,6 +9306,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -9324,7 +9346,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="CaixaDeTexto 8">
@@ -9399,8 +9421,8 @@
       <xdr:row>40</xdr:row>
       <xdr:rowOff>121055</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="CaixaDeTexto 9">
@@ -9449,7 +9471,6 @@
             <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr/>
               <a:r>
                 <a:rPr lang="pt-BR" sz="1100" i="0">
                   <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -9488,7 +9509,7 @@
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
-                          <m:t>[90/-45/0/45]</m:t>
+                          <m:t>[90/−45/0/45]</m:t>
                         </m:r>
                       </m:e>
                       <m:sub>
@@ -9569,7 +9590,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -9582,7 +9603,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -9610,7 +9631,7 @@
                                   <a:schemeClr val="dk1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -9651,7 +9672,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="CaixaDeTexto 9">
@@ -9884,8 +9905,8 @@
       <xdr:rowOff>120046</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="504897" cy="264560"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="CaixaDeTexto 13">
@@ -9927,6 +9948,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -9966,7 +9988,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="CaixaDeTexto 13">
@@ -10041,8 +10063,8 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>173563</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="19" name="CaixaDeTexto 18">
@@ -10091,7 +10113,6 @@
             <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr/>
               <a:r>
                 <a:rPr lang="pt-BR" sz="1100" i="0">
                   <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -10185,7 +10206,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="19" name="CaixaDeTexto 18">
@@ -10866,7 +10887,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="B8:E8"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -11377,8 +11398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4B8029-BC16-4C1F-924A-45DA5A5A793C}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="B6:F6"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
enh: included cross ply case
</commit_message>
<xml_diff>
--- a/multiaxial_plate_optimization/results.xlsx
+++ b/multiaxial_plate_optimization/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\compositeoptimization\multiaxial_plate_optimization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\rafaelmscdissertation\multiaxial_plate_optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2617E1-68AE-47E0-8026-990D4615DD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D4EB8D-8B3D-44E0-9194-1EFF0EC70285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="1" xr2:uid="{FE7EAB9A-19C3-4E00-A1FE-7D328C08052D}"/>
   </bookViews>
@@ -8774,7 +8774,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> and Haftka (1991)</a:t>
+            <a:t> and Haftka (1993)</a:t>
           </a:r>
           <a:endParaRPr lang="pt-BR" sz="1200" b="1">
             <a:solidFill>
@@ -11399,7 +11399,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>